<commit_message>
corrected capm and ff4 models
</commit_message>
<xml_diff>
--- a/dataset_files/ff4_monthly.xlsx
+++ b/dataset_files/ff4_monthly.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andrew\CFM301-FinalProject\dataset_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{277EDC18-4159-4778-B52A-A7FE966173D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CDCD117-2142-4B6D-8EA0-C4097054CB16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,9 +25,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
-    <t>RETX</t>
-  </si>
-  <si>
     <t>SMB</t>
   </si>
   <si>
@@ -41,6 +38,9 @@
   </si>
   <si>
     <t>DATE</t>
+  </si>
+  <si>
+    <t>MKTRF</t>
   </si>
 </sst>
 </file>
@@ -419,9 +419,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F481"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -435,22 +433,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>